<commit_message>
Updated the FILE data object
Renamed the asset data object to FILE.
</commit_message>
<xml_diff>
--- a/2 - Common Metadata Application Profile (MAP)/MOS Common Metadata MAP.xlsx
+++ b/2 - Common Metadata Application Profile (MAP)/MOS Common Metadata MAP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7605" yWindow="-15" windowWidth="7620" windowHeight="10545"/>
+    <workbookView xWindow="7605" yWindow="105" windowWidth="7620" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Public Media MAP for MOS" sheetId="3" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="398">
   <si>
     <t>Array (String)</t>
   </si>
@@ -1073,13 +1073,7 @@
     <t>"TV-PG-V"</t>
   </si>
   <si>
-    <t>5 - Asset</t>
-  </si>
-  <si>
     <t>Maps the file back to a Manifestation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">md:FileDelivery-type .physical </t>
   </si>
   <si>
     <t>Filename on media.
@@ -1516,6 +1510,18 @@
   </si>
   <si>
     <t>manifest, metadata, media, avail, ancillary</t>
+  </si>
+  <si>
+    <t>5 - File</t>
+  </si>
+  <si>
+    <t>mmm:ContentIdentifier-type .Identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmm:FileDelivery-type .physical </t>
+  </si>
+  <si>
+    <t>mmm:AssetPhysicalID-type .Identifier</t>
   </si>
 </sst>
 </file>
@@ -2057,13 +2063,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="78.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2081,7 @@
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="52.7109375" style="15" customWidth="1"/>
     <col min="4" max="4" width="43.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="28" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -2095,7 +2104,7 @@
         <v>94</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>89</v>
@@ -2190,7 +2199,7 @@
         <v>100</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>49</v>
@@ -2209,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>41</v>
@@ -2231,7 +2240,7 @@
 &lt;ID&gt; (domain specific ID) is a string that corresponds with the domain.</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>114</v>
@@ -2265,7 +2274,7 @@
         <v>An organization's GUID (global unique identifier) for internal tracking purposes.</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>114</v>
@@ -2274,7 +2283,7 @@
         <v>67</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>119</v>
@@ -2516,7 +2525,7 @@
         <v>147</v>
       </c>
       <c r="D14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>143</v>
@@ -2543,7 +2552,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>149</v>
@@ -2855,13 +2864,13 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>140</v>
@@ -3055,7 +3064,7 @@
         <v>194</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>193</v>
@@ -3086,7 +3095,7 @@
         <v>196</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>121</v>
@@ -3176,7 +3185,7 @@
         <v>46</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>10</v>
@@ -3210,7 +3219,7 @@
         <v>115</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>114</v>
@@ -3366,7 +3375,7 @@
         <v>56</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="7" t="s">
@@ -3422,10 +3431,10 @@
         <v>46</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>114</v>
@@ -3456,7 +3465,7 @@
         <v>115</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>114</v>
@@ -3692,7 +3701,7 @@
         <v>211</v>
       </c>
       <c r="D52" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>143</v>
@@ -3717,7 +3726,7 @@
         <v>32</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>149</v>
@@ -4090,7 +4099,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" s="3" customFormat="1" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>32</v>
       </c>
@@ -4419,7 +4428,7 @@
         <v>115</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>114</v>
@@ -4449,10 +4458,10 @@
         <v>46</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E76" s="7" t="s">
         <v>114</v>
@@ -4798,19 +4807,19 @@
     </row>
     <row r="87" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
-        <v>260</v>
+        <v>394</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>62</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>114</v>
+        <v>395</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>3</v>
@@ -4829,19 +4838,19 @@
     </row>
     <row r="88" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
-        <v>260</v>
+        <v>394</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>262</v>
+        <v>396</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>3</v>
@@ -4856,26 +4865,26 @@
     </row>
     <row r="89" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
-        <v>260</v>
+        <v>394</v>
       </c>
       <c r="B89" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="D89" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="C89" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>395</v>
-      </c>
       <c r="E89" s="7" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G89" s="8"/>
       <c r="H89" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I89" s="12">
         <v>1</v>
@@ -4889,26 +4898,26 @@
     </row>
     <row r="90" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
-        <v>260</v>
+        <v>394</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>67</v>
       </c>
       <c r="G90" s="8"/>
       <c r="H90" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I90" s="12">
         <v>1</v>
@@ -4922,19 +4931,19 @@
     </row>
     <row r="91" spans="1:11" s="1" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>98</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>7</v>
@@ -4955,16 +4964,16 @@
     </row>
     <row r="92" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>109</v>
@@ -4988,7 +4997,7 @@
     </row>
     <row r="93" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>46</v>
@@ -4997,7 +5006,7 @@
         <v>118</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>114</v>
@@ -5021,13 +5030,13 @@
     </row>
     <row r="94" spans="1:11" s="1" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="7" t="s">
@@ -5052,7 +5061,7 @@
     </row>
     <row r="95" spans="1:11" s="1" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>30</v>
@@ -5085,19 +5094,19 @@
     </row>
     <row r="96" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F96" s="7" t="s">
         <v>74</v>
@@ -5116,10 +5125,10 @@
     </row>
     <row r="97" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C97" s="11" t="str">
         <f>'Data Dictionary'!C6</f>
@@ -5130,13 +5139,13 @@
         <v>Blu-ray, Digital Cinema, Distribution Bundle, DVD, EST, Franchise, Home Entertainment, Syndication, Series, Season:Recut, Season:Pro-Forma, Season:Mini-Series, Other</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="12">
@@ -5151,17 +5160,17 @@
     </row>
     <row r="98" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B98" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C98" s="11" t="s">
         <v>277</v>
-      </c>
-      <c r="C98" s="11" t="s">
-        <v>279</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F98" s="7" t="s">
         <v>80</v>
@@ -5169,7 +5178,7 @@
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
       <c r="I98" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J98" s="7"/>
       <c r="K98" s="7" t="s">
@@ -5178,29 +5187,29 @@
     </row>
     <row r="99" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B99" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C99" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="C99" s="11" t="s">
-        <v>283</v>
-      </c>
       <c r="D99" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F99" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H99" s="8"/>
       <c r="I99" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J99" s="7"/>
       <c r="K99" s="7" t="s">
@@ -5209,13 +5218,13 @@
     </row>
     <row r="100" spans="1:11" s="1" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="7" t="s">
@@ -5292,7 +5301,7 @@
     <hyperlink ref="C93" r:id="rId9" display="cid:org:&lt;Organization URL&gt;:&lt;ID&gt;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="5" scale="52" fitToHeight="0" orientation="landscape" r:id="rId10"/>
   <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
@@ -5335,10 +5344,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="130.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5349,24 +5358,24 @@
         <v>44</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="130.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5385,16 +5394,16 @@
     </row>
     <row r="6" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5405,10 +5414,10 @@
         <v>41</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5419,7 +5428,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>22</v>
@@ -5427,13 +5436,13 @@
     </row>
     <row r="9" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>181</v>
@@ -5447,7 +5456,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>220</v>
@@ -5455,16 +5464,16 @@
     </row>
     <row r="11" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5475,10 +5484,10 @@
         <v>44</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5489,7 +5498,7 @@
         <v>44</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>59</v>
@@ -5503,7 +5512,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>64</v>
@@ -5517,7 +5526,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>83</v>
@@ -5525,51 +5534,51 @@
     </row>
     <row r="16" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D19" s="8"/>
     </row>
@@ -5581,10 +5590,10 @@
         <v>44</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5595,10 +5604,10 @@
         <v>44</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5609,7 +5618,7 @@
         <v>41</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>40</v>
@@ -5617,13 +5626,13 @@
     </row>
     <row r="23" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>18</v>
@@ -5665,7 +5674,7 @@
         <v>44</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>185</v>
@@ -5679,10 +5688,10 @@
         <v>44</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5693,10 +5702,10 @@
         <v>44</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5707,7 +5716,7 @@
         <v>44</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>65</v>
@@ -5724,21 +5733,21 @@
         <v>135</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5749,10 +5758,10 @@
         <v>41</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5777,7 +5786,7 @@
         <v>41</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>127</v>
@@ -5794,7 +5803,7 @@
         <v>138</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5805,38 +5814,38 @@
         <v>41</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5847,7 +5856,7 @@
         <v>41</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>153</v>
@@ -5855,72 +5864,72 @@
     </row>
     <row r="40" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5931,7 +5940,7 @@
         <v>42</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>10</v>
@@ -5945,10 +5954,10 @@
         <v>42</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5959,10 +5968,10 @@
         <v>44</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5973,10 +5982,10 @@
         <v>44</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5987,10 +5996,10 @@
         <v>44</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6015,10 +6024,10 @@
         <v>42</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6029,7 +6038,7 @@
         <v>43</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>171</v>
@@ -6043,7 +6052,7 @@
         <v>43</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>174</v>
@@ -6057,10 +6066,10 @@
         <v>43</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6071,10 +6080,10 @@
         <v>41</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6085,7 +6094,7 @@
         <v>41</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>163</v>
@@ -6099,7 +6108,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>33</v>
@@ -6113,7 +6122,7 @@
         <v>41</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>10</v>
@@ -6192,42 +6201,42 @@
   <sheetData>
     <row r="1" spans="1:3" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>373</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="130.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated the MANIFESTATION label from MANIFEST
</commit_message>
<xml_diff>
--- a/2 - Common Metadata Application Profile (MAP)/MOS Common Metadata MAP.xlsx
+++ b/2 - Common Metadata Application Profile (MAP)/MOS Common Metadata MAP.xlsx
@@ -427,9 +427,6 @@
     <t>Technical</t>
   </si>
   <si>
-    <t>4 - Manifest</t>
-  </si>
-  <si>
     <t>Manifestation UID</t>
   </si>
   <si>
@@ -1522,6 +1519,9 @@
   </si>
   <si>
     <t>mmm:AssetPhysicalID-type .Identifier</t>
+  </si>
+  <si>
+    <t>4 - Manifestation</t>
   </si>
 </sst>
 </file>
@@ -2069,10 +2069,10 @@
   <dimension ref="A1:K119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F102" sqref="F102"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="78.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2092,37 +2092,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="J1" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2130,29 +2130,29 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="12">
         <v>1</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>42</v>
@@ -2163,29 +2163,29 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="12">
         <v>1</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>42</v>
@@ -2196,29 +2196,29 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="12">
         <v>1</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>41</v>
@@ -2240,22 +2240,22 @@
 &lt;ID&gt; (domain specific ID) is a string that corresponds with the domain.</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="I5" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
@@ -2274,25 +2274,25 @@
         <v>An organization's GUID (global unique identifier) for internal tracking purposes.</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I6" s="12">
         <v>1</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>41</v>
@@ -2303,30 +2303,30 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C7" s="11" t="str">
         <f>'Data Dictionary'!C50</f>
         <v>Describes the general type of Series. Most Series are Episodic, which is assumed if no Series Class is provided.</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="12">
         <v>1</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>44</v>
@@ -2337,17 +2337,17 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" s="11" t="str">
         <f>'Data Dictionary'!C34</f>
         <v xml:space="preserve">A mechanism to identify a number's utility. </v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>7</v>
@@ -2367,24 +2367,24 @@
         <v>1</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="15" t="str">
         <f>'Data Dictionary'!C33</f>
         <v xml:space="preserve">Phone number. </v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I9" s="12"/>
       <c r="J9" s="7">
@@ -2399,7 +2399,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" s="11" t="str">
         <f>'Data Dictionary'!C30</f>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>3</v>
@@ -2427,7 +2427,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11" s="11" t="str">
         <f>'Data Dictionary'!C35</f>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>3</v>
@@ -2457,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="11" t="str">
         <f>CONCATENATE("Use when the contactID is blank.", " ",'Data Dictionary'!C32 )</f>
@@ -2465,14 +2465,14 @@
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I12" s="12">
         <v>1</v>
@@ -2489,7 +2489,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C13" s="11" t="str">
         <f>CONCATENATE("If an existing contact is reused, provide the contactID and leave the remaining contact fields blank.",'Data Dictionary'!C31)</f>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>7</v>
@@ -2508,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>41</v>
@@ -2519,29 +2519,29 @@
         <v>1</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>147</v>
-      </c>
       <c r="D14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="12">
         <v>0</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>41</v>
@@ -2552,16 +2552,16 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>150</v>
-      </c>
       <c r="E15" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>7</v>
@@ -2581,22 +2581,22 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="12">
@@ -2612,16 +2612,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>4</v>
@@ -2629,10 +2629,10 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>41</v>
@@ -2646,24 +2646,24 @@
         <v>47</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="12">
         <v>1</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>41</v>
@@ -2674,29 +2674,29 @@
         <v>1</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="12">
         <v>1</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>41</v>
@@ -2710,13 +2710,13 @@
         <v>14</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>3</v>
@@ -2727,7 +2727,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>43</v>
@@ -2741,19 +2741,19 @@
         <v>21</v>
       </c>
       <c r="C21" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>166</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>167</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>11</v>
@@ -2762,7 +2762,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>43</v>
@@ -2776,16 +2776,16 @@
         <v>13</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>171</v>
-      </c>
       <c r="E22" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -2805,16 +2805,16 @@
         <v>26</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>174</v>
-      </c>
       <c r="E23" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -2831,29 +2831,29 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="12">
         <v>1</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>41</v>
@@ -2864,29 +2864,29 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>43</v>
@@ -2897,29 +2897,29 @@
         <v>1</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="E26" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>43</v>
@@ -2933,23 +2933,23 @@
         <v>36</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="7" t="s">
@@ -2961,27 +2961,27 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>187</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="12">
         <v>1</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>44</v>
@@ -2995,26 +2995,26 @@
         <v>34</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="12">
         <v>1</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>44</v>
@@ -3025,16 +3025,16 @@
         <v>1</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>3</v>
@@ -3047,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>44</v>
@@ -3061,13 +3061,13 @@
         <v>30</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>3</v>
@@ -3075,10 +3075,10 @@
       <c r="G31" s="8"/>
       <c r="H31" s="17"/>
       <c r="I31" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>44</v>
@@ -3089,29 +3089,29 @@
         <v>27</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>196</v>
-      </c>
       <c r="D32" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="12">
         <v>1</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>44</v>
@@ -3122,29 +3122,29 @@
         <v>27</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="12">
         <v>1</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>42</v>
@@ -3158,11 +3158,11 @@
         <v>56</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>3</v>
@@ -3185,20 +3185,20 @@
         <v>46</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I35" s="12">
         <v>1</v>
@@ -3216,25 +3216,25 @@
         <v>2</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G36" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H36" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H36" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="I36" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J36" s="7"/>
       <c r="K36" s="7" t="s">
@@ -3255,7 +3255,7 @@
         <v>51</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>3</v>
@@ -3266,7 +3266,7 @@
         <v>1</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>43</v>
@@ -3277,19 +3277,19 @@
         <v>27</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -3309,13 +3309,13 @@
         <v>30</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>3</v>
@@ -3328,7 +3328,7 @@
         <v>1</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K39" s="7" t="s">
         <v>44</v>
@@ -3339,29 +3339,29 @@
         <v>32</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C40" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="E40" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H40" s="8"/>
       <c r="I40" s="12">
         <v>1</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K40" s="7" t="s">
         <v>42</v>
@@ -3375,11 +3375,11 @@
         <v>56</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>0</v>
@@ -3402,13 +3402,13 @@
         <v>6</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>3</v>
@@ -3431,20 +3431,20 @@
         <v>46</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I43" s="12">
         <v>1</v>
@@ -3462,25 +3462,25 @@
         <v>2</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G44" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H44" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H44" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="I44" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J44" s="7"/>
       <c r="K44" s="7" t="s">
@@ -3495,26 +3495,26 @@
         <v>54</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>55</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="12">
         <v>1</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K45" s="7" t="s">
         <v>44</v>
@@ -3525,14 +3525,14 @@
         <v>32</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>7</v>
@@ -3552,26 +3552,26 @@
         <v>32</v>
       </c>
       <c r="B47" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J47" s="7"/>
       <c r="K47" s="7" t="s">
@@ -3583,14 +3583,14 @@
         <v>32</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>3</v>
@@ -3610,14 +3610,14 @@
         <v>32</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>3</v>
@@ -3637,21 +3637,21 @@
         <v>32</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I50" s="12">
         <v>1</v>
@@ -3666,14 +3666,14 @@
         <v>32</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>7</v>
@@ -3684,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K51" s="7" t="s">
         <v>41</v>
@@ -3695,27 +3695,27 @@
         <v>32</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D52" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H52" s="8"/>
       <c r="I52" s="12"/>
       <c r="J52" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K52" s="7" t="s">
         <v>41</v>
@@ -3726,16 +3726,16 @@
         <v>32</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C53" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="8" t="s">
-        <v>150</v>
-      </c>
       <c r="E53" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>7</v>
@@ -3755,22 +3755,22 @@
         <v>32</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="12">
@@ -3786,14 +3786,14 @@
         <v>32</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>4</v>
@@ -3801,10 +3801,10 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
       <c r="I55" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K55" s="7" t="s">
         <v>41</v>
@@ -3818,24 +3818,24 @@
         <v>47</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H56" s="8"/>
       <c r="I56" s="12">
         <v>1</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K56" s="7" t="s">
         <v>44</v>
@@ -3849,16 +3849,16 @@
         <v>14</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
@@ -3866,7 +3866,7 @@
         <v>1</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K57" s="7" t="s">
         <v>43</v>
@@ -3880,16 +3880,16 @@
         <v>45</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
@@ -3909,19 +3909,19 @@
         <v>21</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H59" s="8" t="s">
         <v>11</v>
@@ -3930,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K59" s="7" t="s">
         <v>43</v>
@@ -3941,29 +3941,29 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
+        <v>174</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H60" s="8"/>
       <c r="I60" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K60" s="7" t="s">
         <v>41</v>
@@ -3974,29 +3974,29 @@
         <v>32</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D61" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C61" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="E61" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G61" s="8"/>
       <c r="H61" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I61" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="J61" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="J61" s="7" t="s">
-        <v>223</v>
       </c>
       <c r="K61" s="7" t="s">
         <v>43</v>
@@ -4010,13 +4010,13 @@
         <v>52</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>7</v>
@@ -4029,7 +4029,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K62" s="7" t="s">
         <v>43</v>
@@ -4043,26 +4043,26 @@
         <v>24</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H63" s="8"/>
       <c r="I63" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K63" s="7" t="s">
         <v>43</v>
@@ -4076,16 +4076,16 @@
         <v>13</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
@@ -4093,7 +4093,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K64" s="7" t="s">
         <v>43</v>
@@ -4107,16 +4107,16 @@
         <v>26</v>
       </c>
       <c r="C65" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D65" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="D65" s="8" t="s">
-        <v>231</v>
-      </c>
       <c r="E65" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
@@ -4124,7 +4124,7 @@
         <v>1</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K65" s="7" t="s">
         <v>43</v>
@@ -4135,16 +4135,16 @@
         <v>32</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>3</v>
@@ -4157,7 +4157,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K66" s="7" t="s">
         <v>44</v>
@@ -4168,19 +4168,19 @@
         <v>32</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
@@ -4188,7 +4188,7 @@
         <v>1</v>
       </c>
       <c r="J67" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K67" s="7" t="s">
         <v>44</v>
@@ -4199,19 +4199,19 @@
         <v>32</v>
       </c>
       <c r="B68" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D68" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C68" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="E68" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
@@ -4219,7 +4219,7 @@
         <v>1</v>
       </c>
       <c r="J68" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K68" s="7" t="s">
         <v>44</v>
@@ -4233,23 +4233,23 @@
         <v>36</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H69" s="8"/>
       <c r="I69" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J69" s="7"/>
       <c r="K69" s="7" t="s">
@@ -4261,27 +4261,27 @@
         <v>32</v>
       </c>
       <c r="B70" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>187</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H70" s="17"/>
       <c r="I70" s="12">
         <v>1</v>
       </c>
       <c r="J70" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K70" s="7" t="s">
         <v>44</v>
@@ -4295,19 +4295,19 @@
         <v>34</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H71" s="8" t="s">
         <v>11</v>
@@ -4316,7 +4316,7 @@
         <v>1</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K71" s="7" t="s">
         <v>44</v>
@@ -4330,13 +4330,13 @@
         <v>30</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>3</v>
@@ -4349,7 +4349,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K72" s="7" t="s">
         <v>44</v>
@@ -4357,25 +4357,25 @@
     </row>
     <row r="73" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H73" s="8"/>
       <c r="I73" s="12">
@@ -4388,19 +4388,19 @@
     </row>
     <row r="74" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>3</v>
@@ -4411,7 +4411,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K74" s="7" t="s">
         <v>42</v>
@@ -4419,31 +4419,31 @@
     </row>
     <row r="75" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G75" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H75" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H75" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="I75" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J75" s="7"/>
       <c r="K75" s="7" t="s">
@@ -4452,32 +4452,32 @@
     </row>
     <row r="76" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G76" s="8"/>
       <c r="H76" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I76" s="12">
         <v>1</v>
       </c>
       <c r="J76" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K76" s="7" t="s">
         <v>41</v>
@@ -4485,19 +4485,19 @@
     </row>
     <row r="77" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>16</v>
@@ -4507,10 +4507,10 @@
         <v>17</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K77" s="7" t="s">
         <v>44</v>
@@ -4518,19 +4518,19 @@
     </row>
     <row r="78" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E78" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>16</v>
@@ -4540,10 +4540,10 @@
         <v>17</v>
       </c>
       <c r="I78" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J78" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K78" s="7" t="s">
         <v>44</v>
@@ -4551,32 +4551,32 @@
     </row>
     <row r="79" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H79" s="8"/>
       <c r="I79" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J79" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K79" s="7" t="s">
         <v>44</v>
@@ -4584,29 +4584,29 @@
     </row>
     <row r="80" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>59</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H80" s="8"/>
       <c r="I80" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J80" s="7"/>
       <c r="K80" s="7" t="s">
@@ -4615,19 +4615,19 @@
     </row>
     <row r="81" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>3</v>
@@ -4646,19 +4646,19 @@
     </row>
     <row r="82" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>3</v>
@@ -4671,7 +4671,7 @@
         <v>1</v>
       </c>
       <c r="J82" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K82" s="7" t="s">
         <v>44</v>
@@ -4679,19 +4679,19 @@
     </row>
     <row r="83" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>3</v>
@@ -4710,19 +4710,19 @@
     </row>
     <row r="84" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F84" s="7" t="s">
         <v>3</v>
@@ -4733,7 +4733,7 @@
         <v>1</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K84" s="7" t="s">
         <v>43</v>
@@ -4741,25 +4741,25 @@
     </row>
     <row r="85" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H85" s="8" t="s">
         <v>11</v>
@@ -4774,32 +4774,32 @@
     </row>
     <row r="86" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
-        <v>61</v>
+        <v>397</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E86" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F86" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H86" s="8"/>
       <c r="I86" s="12">
         <v>1</v>
       </c>
       <c r="J86" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K86" s="7" t="s">
         <v>60</v>
@@ -4807,19 +4807,19 @@
     </row>
     <row r="87" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>3</v>
@@ -4830,7 +4830,7 @@
         <v>1</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K87" s="7" t="s">
         <v>42</v>
@@ -4838,19 +4838,19 @@
     </row>
     <row r="88" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>3</v>
@@ -4865,32 +4865,32 @@
     </row>
     <row r="89" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B89" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C89" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="D89" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="D89" s="8" t="s">
-        <v>393</v>
-      </c>
       <c r="E89" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G89" s="8"/>
       <c r="H89" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I89" s="12">
         <v>1</v>
       </c>
       <c r="J89" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K89" s="7" t="s">
         <v>44</v>
@@ -4898,32 +4898,32 @@
     </row>
     <row r="90" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G90" s="8"/>
       <c r="H90" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I90" s="12">
         <v>1</v>
       </c>
       <c r="J90" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K90" s="7" t="s">
         <v>41</v>
@@ -4931,32 +4931,32 @@
     </row>
     <row r="91" spans="1:11" s="1" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E91" s="7" t="s">
         <v>262</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>263</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H91" s="8"/>
       <c r="I91" s="12">
         <v>1</v>
       </c>
       <c r="J91" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K91" s="7" t="s">
         <v>42</v>
@@ -4964,32 +4964,32 @@
     </row>
     <row r="92" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G92" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H92" s="8"/>
       <c r="I92" s="12">
         <v>1</v>
       </c>
       <c r="J92" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K92" s="7" t="s">
         <v>42</v>
@@ -4997,32 +4997,32 @@
     </row>
     <row r="93" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G93" s="8"/>
       <c r="H93" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I93" s="12">
         <v>1</v>
       </c>
       <c r="J93" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K93" s="7" t="s">
         <v>41</v>
@@ -5030,29 +5030,29 @@
     </row>
     <row r="94" spans="1:11" s="1" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B94" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C94" s="11" t="s">
         <v>268</v>
-      </c>
-      <c r="C94" s="11" t="s">
-        <v>269</v>
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G94" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H94" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H94" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="I94" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J94" s="7"/>
       <c r="K94" s="7" t="s">
@@ -5061,19 +5061,19 @@
     </row>
     <row r="95" spans="1:11" s="1" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>3</v>
@@ -5086,7 +5086,7 @@
         <v>1</v>
       </c>
       <c r="J95" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K95" s="7" t="s">
         <v>44</v>
@@ -5094,22 +5094,22 @@
     </row>
     <row r="96" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C96" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="D96" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="D96" s="8" t="s">
-        <v>272</v>
-      </c>
       <c r="E96" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
@@ -5117,7 +5117,7 @@
         <v>1</v>
       </c>
       <c r="J96" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K96" s="7" t="s">
         <v>43</v>
@@ -5125,10 +5125,10 @@
     </row>
     <row r="97" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C97" s="11" t="str">
         <f>'Data Dictionary'!C6</f>
@@ -5139,20 +5139,20 @@
         <v>Blu-ray, Digital Cinema, Distribution Bundle, DVD, EST, Franchise, Home Entertainment, Syndication, Series, Season:Recut, Season:Pro-Forma, Season:Mini-Series, Other</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H97" s="8"/>
       <c r="I97" s="12">
         <v>1</v>
       </c>
       <c r="J97" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K97" s="7" t="s">
         <v>44</v>
@@ -5160,25 +5160,25 @@
     </row>
     <row r="98" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
       <c r="I98" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J98" s="7"/>
       <c r="K98" s="7" t="s">
@@ -5187,29 +5187,29 @@
     </row>
     <row r="99" spans="1:11" s="3" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B99" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E99" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>280</v>
       </c>
       <c r="F99" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H99" s="8"/>
       <c r="I99" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J99" s="7"/>
       <c r="K99" s="7" t="s">
@@ -5218,26 +5218,26 @@
     </row>
     <row r="100" spans="1:11" s="1" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G100" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H100" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="H100" s="8" t="s">
-        <v>117</v>
       </c>
       <c r="I100" s="12">
         <v>1</v>
@@ -5324,69 +5324,69 @@
   <sheetData>
     <row r="1" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>340</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="130.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="130.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>12</v>
@@ -5394,16 +5394,16 @@
     </row>
     <row r="6" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5414,10 +5414,10 @@
         <v>41</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5428,7 +5428,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>22</v>
@@ -5436,58 +5436,58 @@
     </row>
     <row r="9" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5498,7 +5498,7 @@
         <v>44</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>59</v>
@@ -5512,10 +5512,10 @@
         <v>44</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5526,59 +5526,59 @@
         <v>41</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D19" s="8"/>
     </row>
@@ -5590,24 +5590,24 @@
         <v>44</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>350</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5618,7 +5618,7 @@
         <v>41</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>40</v>
@@ -5626,13 +5626,13 @@
     </row>
     <row r="23" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>18</v>
@@ -5646,7 +5646,7 @@
         <v>43</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>9</v>
@@ -5660,7 +5660,7 @@
         <v>43</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>25</v>
@@ -5674,24 +5674,24 @@
         <v>44</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>329</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5702,234 +5702,234 @@
         <v>44</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>368</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5940,7 +5940,7 @@
         <v>42</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>10</v>
@@ -5948,16 +5948,16 @@
     </row>
     <row r="46" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5968,66 +5968,66 @@
         <v>44</v>
       </c>
       <c r="C47" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>338</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6038,10 +6038,10 @@
         <v>43</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6052,10 +6052,10 @@
         <v>43</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6066,10 +6066,10 @@
         <v>43</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6080,24 +6080,24 @@
         <v>41</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6108,7 +6108,7 @@
         <v>43</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>33</v>
@@ -6122,7 +6122,7 @@
         <v>41</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>10</v>
@@ -6136,7 +6136,7 @@
         <v>44</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>18</v>
@@ -6150,7 +6150,7 @@
         <v>44</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>18</v>
@@ -6158,16 +6158,16 @@
     </row>
     <row r="61" spans="1:4" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -6201,42 +6201,42 @@
   <sheetData>
     <row r="1" spans="1:3" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>372</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="130.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>377</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>